<commit_message>
added illustrative chart and co2 estimates
</commit_message>
<xml_diff>
--- a/data/electric-uptake.xlsx
+++ b/data/electric-uptake.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lffox/Dropbox (Grattan Institute)/Transport Program/Project - Trucks/Analysis/truck-modelling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B253C4BD-5C65-F841-8BED-76314D9840B4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62903CD3-3862-EE43-B23B-C0692601E05E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6352,7 +6352,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6385,7 +6385,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6399,7 +6399,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -6414,7 +6414,7 @@
         <v>7.5</v>
       </c>
       <c r="D4" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -6428,7 +6428,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -6443,7 +6443,7 @@
         <v>16.666666666666668</v>
       </c>
       <c r="D6" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -6458,7 +6458,7 @@
         <v>23.333333333333336</v>
       </c>
       <c r="D7" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -6472,7 +6472,7 @@
         <v>30</v>
       </c>
       <c r="D8" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -6487,7 +6487,7 @@
         <v>36</v>
       </c>
       <c r="D9" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -6502,7 +6502,7 @@
         <v>42</v>
       </c>
       <c r="D10" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -6517,7 +6517,7 @@
         <v>48</v>
       </c>
       <c r="D11" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -6532,7 +6532,7 @@
         <v>54</v>
       </c>
       <c r="D12" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -6546,7 +6546,7 @@
         <v>60</v>
       </c>
       <c r="D13" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -6561,7 +6561,7 @@
         <v>68</v>
       </c>
       <c r="D14" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -6576,7 +6576,7 @@
         <v>76</v>
       </c>
       <c r="D15" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -6591,7 +6591,7 @@
         <v>84</v>
       </c>
       <c r="D16" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -6606,7 +6606,7 @@
         <v>92</v>
       </c>
       <c r="D17" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -6620,7 +6620,7 @@
         <v>100</v>
       </c>
       <c r="D18" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -6634,7 +6634,7 @@
         <v>1</v>
       </c>
       <c r="D19" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -6645,10 +6645,10 @@
         <v>2025</v>
       </c>
       <c r="C20">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="D20" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -6659,10 +6659,10 @@
         <v>2026</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D21" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -6673,10 +6673,10 @@
         <v>2027</v>
       </c>
       <c r="C22">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D22" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -6687,10 +6687,10 @@
         <v>2028</v>
       </c>
       <c r="C23" s="4">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D23" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -6701,10 +6701,10 @@
         <v>2029</v>
       </c>
       <c r="C24" s="4">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D24" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -6715,10 +6715,10 @@
         <v>2030</v>
       </c>
       <c r="C25">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D25" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -6729,10 +6729,10 @@
         <v>2031</v>
       </c>
       <c r="C26">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D26" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -6743,10 +6743,10 @@
         <v>2032</v>
       </c>
       <c r="C27">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D27" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -6757,10 +6757,10 @@
         <v>2033</v>
       </c>
       <c r="C28">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D28" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -6771,10 +6771,10 @@
         <v>2034</v>
       </c>
       <c r="C29">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D29" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -6785,10 +6785,10 @@
         <v>2035</v>
       </c>
       <c r="C30">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="D30" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -6799,10 +6799,10 @@
         <v>2036</v>
       </c>
       <c r="C31">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D31" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -6813,10 +6813,10 @@
         <v>2037</v>
       </c>
       <c r="C32">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="D32" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -6827,10 +6827,10 @@
         <v>2038</v>
       </c>
       <c r="C33">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D33" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -6841,10 +6841,10 @@
         <v>2039</v>
       </c>
       <c r="C34">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="D34" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -6855,10 +6855,10 @@
         <v>2040</v>
       </c>
       <c r="C35">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="D35" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>